<commit_message>
Nuevas hojas de trabajo más tabla hecha con los fundamentos basicos de Excel, ademas de nuevo archivo pdf del formato de impresión del documento
</commit_message>
<xml_diff>
--- a/Mi primer Excel.xlsx
+++ b/Mi primer Excel.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juans\OneDrive\Escritorio\Platzi\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CCE69D-FB66-40D8-9DDC-D7B4B06B0EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF6852A-9BE8-41E0-9E78-70132466398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4984995E-A29E-4F3B-A8E9-0B6562FC4525}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Ventas" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Vista para impresión" guid="{BCFC9ACA-0DA4-40CC-B384-1B6FFB461E1B}" xWindow="953" windowWidth="974" windowHeight="1039" activeSheetId="3"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,9 +40,57 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Platzi</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Empresa 1</t>
+  </si>
+  <si>
+    <t>Empresa 2</t>
+  </si>
+  <si>
+    <t>Empresa 3</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Monto vendido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +98,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF99FF"/>
+      <name val="Chiller"/>
+      <family val="5"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Amasis MT Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5"/>
+      <name val="Brush Script MT"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Curlz MT"/>
+      <family val="5"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,17 +167,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -402,12 +528,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85BDCC0-3E2A-4791-9CBC-D46253FFE3D3}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>555555</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9">
+        <v>555555</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>777777</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="5">
+        <v>777777</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>999999</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7">
+        <v>888888</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="7">
+        <v>888888</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>555555</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>777777</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>999999</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="9">
+        <v>555555</v>
+      </c>
+      <c r="K11" s="5">
+        <v>777777</v>
+      </c>
+      <c r="L11" s="6">
+        <v>999999</v>
+      </c>
+      <c r="M11" s="7">
+        <v>888888</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>888888</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{BCFC9ACA-0DA4-40CC-B384-1B6FFB461E1B}" scale="160" showPageBreaks="1" view="pageBreakPreview">
+      <selection activeCell="D9" sqref="D9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="77" orientation="landscape" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCD7110-E9AE-49BD-9A89-BDC13B9C8742}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>44562</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{BCFC9ACA-0DA4-40CC-B384-1B6FFB461E1B}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F792ACD6-877A-474F-80DD-6C22E52DC7B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <customSheetViews>
+    <customSheetView guid="{BCFC9ACA-0DA4-40CC-B384-1B6FFB461E1B}" showPageBreaks="1" view="pageLayout">
+      <selection activeCell="B2" sqref="B2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <headerFooter>
+        <oddHeader>&amp;CVentas Mensuales</oddHeader>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;CVentas Mensuales</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificaciones de Mi primer Excel, añadición de archivo de atajos de teclado en Excel ademas de una carpeta de recursos para el desarrollo del curso, por ultimo el archivo .gitignore para los archivo binarios
</commit_message>
<xml_diff>
--- a/Mi primer Excel.xlsx
+++ b/Mi primer Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juans\OneDrive\Escritorio\Platzi\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF6852A-9BE8-41E0-9E78-70132466398E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA68467-7F73-4337-9802-12B7871FB303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4984995E-A29E-4F3B-A8E9-0B6562FC4525}"/>
   </bookViews>
@@ -40,21 +40,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={CEBC27CD-B9A6-4395-8AE1-B8527A877613}</author>
+    <author>tc={C679515A-1B4F-488E-BE17-E02A2BA7BC05}</author>
+    <author>tc={69E16F1C-49B8-4E10-9E5E-EC3BB4FDA857}</author>
+    <author>tc={EA16A05F-15DB-4A70-8D67-9342DF33BC19}</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{CEBC27CD-B9A6-4395-8AE1-B8527A877613}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Cambiar color</t>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="1" shapeId="0" xr:uid="{C679515A-1B4F-488E-BE17-E02A2BA7BC05}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    La mejor empresa del mundo!!!</t>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="2" shapeId="0" xr:uid="{69E16F1C-49B8-4E10-9E5E-EC3BB4FDA857}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Ya no es nuestro cliente</t>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="3" shapeId="0" xr:uid="{EA16A05F-15DB-4A70-8D67-9342DF33BC19}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Laura cambió de teléfono</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
-    <t>Benjamin</t>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
     <t>Luis</t>
   </si>
   <si>
-    <t>Telefono</t>
-  </si>
-  <si>
     <t>Platzi</t>
   </si>
   <si>
@@ -80,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ana </t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Benjamín</t>
   </si>
 </sst>
 </file>
@@ -88,9 +133,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +188,12 @@
       <name val="Curlz MT"/>
       <family val="5"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -171,11 +222,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -209,6 +259,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sebas Bustos" id="{865E748B-BE60-44FE-84CD-84752CC32763}" userId="Sebas Bustos" providerId="None"/>
+  <person displayName="JUAN SEBASTIAN BUSTOS RUIZ" id="{CDFCDA2E-FC07-4F88-95DC-6C253A0D8782}" userId="S::juansbustos@ucundinamarca.edu.co::86cde44e-f9a3-4ac0-8bec-d208c6639716" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,227 +583,240 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" personId="{865E748B-BE60-44FE-84CD-84752CC32763}" id="{CEBC27CD-B9A6-4395-8AE1-B8527A877613}">
+    <text>Cambiar color</text>
+  </threadedComment>
+  <threadedComment ref="C3" personId="{865E748B-BE60-44FE-84CD-84752CC32763}" id="{C679515A-1B4F-488E-BE17-E02A2BA7BC05}">
+    <text>La mejor empresa del mundo!!!</text>
+  </threadedComment>
+  <threadedComment ref="B4" dT="2024-06-12T15:17:35.09" personId="{CDFCDA2E-FC07-4F88-95DC-6C253A0D8782}" id="{69E16F1C-49B8-4E10-9E5E-EC3BB4FDA857}">
+    <text>Ya no es nuestro cliente</text>
+  </threadedComment>
+  <threadedComment ref="D5" dT="2024-06-12T15:18:36.29" personId="{CDFCDA2E-FC07-4F88-95DC-6C253A0D8782}" id="{EA16A05F-15DB-4A70-8D67-9342DF33BC19}">
+    <text>Laura cambió de teléfono</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85BDCC0-3E2A-4791-9CBC-D46253FFE3D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85BDCC0-3E2A-4791-9CBC-D46253FFE3D3}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M12"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
     <row r="2" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>555555</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <v>555555</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>777777</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>777777</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="D5" s="5">
+        <v>999999</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="9">
-        <v>555555</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9">
-        <v>555555</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="H5" s="5">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5">
-        <v>777777</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="D6" s="6">
+        <v>888888</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5">
-        <v>777777</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6">
-        <v>999999</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="6">
-        <v>999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7">
-        <v>888888</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>888888</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>555555</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>1</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>777777</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="I10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>999999</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="9">
+      <c r="I11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="8">
         <v>555555</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>777777</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>999999</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>888888</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>888888</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatRows="0" sort="0"/>
   <customSheetViews>
     <customSheetView guid="{BCFC9ACA-0DA4-40CC-B384-1B6FFB461E1B}" scale="160" showPageBreaks="1" view="pageBreakPreview">
       <selection activeCell="D9" sqref="D9"/>
@@ -757,6 +827,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="77" orientation="landscape" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -777,17 +848,17 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>44562</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1200</v>
       </c>
     </row>
@@ -806,9 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F792ACD6-877A-474F-80DD-6C22E52DC7B7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>